<commit_message>
Results from July 29, 2020 03:07:37 PM America/Los_Angeles TZ run
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-29.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-29.xlsx
@@ -1042,20 +1042,20 @@
         </is>
       </c>
       <c r="B13" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C13" t="n">
-        <v>19791</v>
+        <v>20136</v>
       </c>
       <c r="D13" t="n">
-        <v>626</v>
+        <v>632</v>
       </c>
       <c r="E13" t="n">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="F13" t="inlineStr"/>
       <c r="G13" t="n">
-        <v>1.88</v>
+        <v>1.86</v>
       </c>
       <c r="H13" t="inlineStr"/>
       <c r="I13" t="b">
@@ -1716,13 +1716,13 @@
         </is>
       </c>
       <c r="B27" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C27" t="n">
-        <v>45314</v>
+        <v>45796</v>
       </c>
       <c r="D27" t="n">
-        <v>1807</v>
+        <v>1822</v>
       </c>
       <c r="E27" t="n">
         <v>2130</v>
@@ -1731,10 +1731,10 @@
         <v>121</v>
       </c>
       <c r="G27" t="n">
-        <v>6.07</v>
+        <v>6.02</v>
       </c>
       <c r="H27" t="n">
-        <v>6.93</v>
+        <v>6.87</v>
       </c>
       <c r="I27" t="b">
         <v>0</v>
@@ -1743,10 +1743,10 @@
         <v>0</v>
       </c>
       <c r="K27" t="n">
-        <v>35069</v>
+        <v>35396</v>
       </c>
       <c r="L27" t="n">
-        <v>1745</v>
+        <v>1761</v>
       </c>
       <c r="M27" t="n">
         <v>227938</v>
@@ -2214,25 +2214,25 @@
         </is>
       </c>
       <c r="B37" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C37" t="n">
-        <v>6500</v>
+        <v>6513</v>
       </c>
       <c r="D37" t="n">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="E37" t="n">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="F37" t="n">
         <v>9</v>
       </c>
       <c r="G37" t="n">
-        <v>5.99</v>
+        <v>5.98</v>
       </c>
       <c r="H37" t="n">
-        <v>2.22</v>
+        <v>2.21</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
@@ -2241,10 +2241,10 @@
         <v>0</v>
       </c>
       <c r="K37" t="n">
-        <v>5630</v>
+        <v>5650</v>
       </c>
       <c r="L37" t="n">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="M37" t="n">
         <v>20516</v>
@@ -2581,39 +2581,21 @@
           <t>Ohio</t>
         </is>
       </c>
-      <c r="B45" s="2" t="n">
-        <v>44041</v>
-      </c>
-      <c r="C45" t="n">
-        <v>87893</v>
-      </c>
-      <c r="D45" t="n">
-        <v>3422</v>
-      </c>
-      <c r="E45" t="n">
-        <v>22203</v>
-      </c>
-      <c r="F45" t="n">
-        <v>657</v>
-      </c>
-      <c r="G45" t="n">
-        <v>29.2</v>
-      </c>
-      <c r="H45" t="n">
-        <v>19.57</v>
-      </c>
+      <c r="B45" t="inlineStr"/>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
+      <c r="E45" t="inlineStr"/>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="b">
-        <v>1</v>
-      </c>
-      <c r="K45" t="n">
-        <v>76047</v>
-      </c>
-      <c r="L45" t="n">
-        <v>3357</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
       <c r="M45" t="n">
         <v>1438271</v>
       </c>
@@ -2622,7 +2604,7 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Results from 2020-07-29 9:30 PM CT
</commit_message>
<xml_diff>
--- a/workflow/python/output/xlsx/covid_disparities_output_2020-07-29.xlsx
+++ b/workflow/python/output/xlsx/covid_disparities_output_2020-07-29.xlsx
@@ -73,74 +73,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -433,7 +365,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O53"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,29 +453,29 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Texas</t>
+          <t>Illinois</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C2" t="n">
-        <v>33857</v>
+        <v>175124</v>
       </c>
       <c r="D2" t="n">
-        <v>6190</v>
+        <v>7462</v>
       </c>
       <c r="E2" t="n">
-        <v>4442</v>
+        <v>29105</v>
       </c>
       <c r="F2" t="n">
-        <v>866</v>
+        <v>2045</v>
       </c>
       <c r="G2" t="n">
-        <v>13.12</v>
+        <v>16.62</v>
       </c>
       <c r="H2" t="n">
-        <v>13.99</v>
+        <v>27.41</v>
       </c>
       <c r="I2" t="b">
         <v>1</v>
@@ -554,10 +486,10 @@
       <c r="K2" t="inlineStr"/>
       <c r="L2" t="inlineStr"/>
       <c r="M2" t="n">
-        <v>3365783</v>
+        <v>1824125</v>
       </c>
       <c r="N2" t="n">
-        <v>12.07</v>
+        <v>14.23</v>
       </c>
       <c r="O2" t="inlineStr">
         <is>
@@ -568,47 +500,47 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Texas -- Bexar County</t>
+          <t>Louisiana</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C3" t="n">
-        <v>37984</v>
+        <v>112773</v>
       </c>
       <c r="D3" t="n">
-        <v>335</v>
+        <v>3769</v>
       </c>
       <c r="E3" t="n">
-        <v>464</v>
+        <v>41962</v>
       </c>
       <c r="F3" t="n">
-        <v>17</v>
+        <v>1884</v>
       </c>
       <c r="G3" t="n">
-        <v>6.81</v>
+        <v>44.38</v>
       </c>
       <c r="H3" t="n">
-        <v>15.32</v>
+        <v>50.36</v>
       </c>
       <c r="I3" t="b">
         <v>0</v>
       </c>
       <c r="J3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3" t="n">
-        <v>6812</v>
+        <v>94556</v>
       </c>
       <c r="L3" t="n">
-        <v>111</v>
+        <v>3741</v>
       </c>
       <c r="M3" t="n">
-        <v>146703</v>
+        <v>1502916</v>
       </c>
       <c r="N3" t="n">
-        <v>7.62</v>
+        <v>32.23</v>
       </c>
       <c r="O3" t="inlineStr">
         <is>
@@ -619,51 +551,47 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>New York -- New York</t>
+          <t>Washington</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
         <v>44041</v>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>221220</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>18887</t>
-        </is>
+      <c r="C4" t="n">
+        <v>54985</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1555</v>
       </c>
       <c r="E4" t="n">
-        <v>34191</v>
+        <v>2042</v>
       </c>
       <c r="F4" t="n">
-        <v>5267</v>
+        <v>49</v>
       </c>
       <c r="G4" t="n">
-        <v>29.91</v>
+        <v>5.5</v>
       </c>
       <c r="H4" t="n">
-        <v>30.45</v>
+        <v>3.23</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>114310</v>
+        <v>37156</v>
       </c>
       <c r="L4" t="n">
-        <v>17298</v>
+        <v>1517</v>
       </c>
       <c r="M4" t="n">
-        <v>2049418</v>
+        <v>269854</v>
       </c>
       <c r="N4" t="n">
-        <v>24.27</v>
+        <v>3.7</v>
       </c>
       <c r="O4" t="inlineStr">
         <is>
@@ -674,47 +602,47 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Rhode Island</t>
+          <t>North Carolina</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44015</v>
+        <v>44041</v>
       </c>
       <c r="C5" t="n">
-        <v>16491</v>
+        <v>117850</v>
       </c>
       <c r="D5" t="n">
-        <v>960</v>
+        <v>1865</v>
       </c>
       <c r="E5" t="n">
-        <v>1592</v>
+        <v>20252</v>
       </c>
       <c r="F5" t="n">
-        <v>48</v>
+        <v>576</v>
       </c>
       <c r="G5" t="n">
-        <v>12.29</v>
+        <v>24.04</v>
       </c>
       <c r="H5" t="n">
-        <v>6.14</v>
+        <v>31.96</v>
       </c>
       <c r="I5" t="b">
         <v>0</v>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5" t="n">
-        <v>12950</v>
+        <v>84258</v>
       </c>
       <c r="L5" t="n">
-        <v>782</v>
+        <v>1802</v>
       </c>
       <c r="M5" t="n">
-        <v>69254</v>
+        <v>2179622</v>
       </c>
       <c r="N5" t="n">
-        <v>6.55</v>
+        <v>21.46</v>
       </c>
       <c r="O5" t="inlineStr">
         <is>
@@ -725,83 +653,87 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>California - San Francisco</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr"/>
-      <c r="D6" t="inlineStr"/>
-      <c r="E6" t="inlineStr"/>
-      <c r="F6" t="inlineStr"/>
-      <c r="G6" t="inlineStr"/>
-      <c r="H6" t="inlineStr"/>
+          <t>Wyoming</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>44041</v>
+      </c>
+      <c r="C6" t="n">
+        <v>2628</v>
+      </c>
+      <c r="D6" t="n">
+        <v>26</v>
+      </c>
+      <c r="E6" t="n">
+        <v>27</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>1.06</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0</v>
+      </c>
       <c r="I6" t="b">
         <v>0</v>
       </c>
       <c r="J6" t="b">
         <v>0</v>
       </c>
-      <c r="K6" t="inlineStr"/>
-      <c r="L6" t="inlineStr"/>
-      <c r="M6" t="inlineStr"/>
-      <c r="N6" t="inlineStr"/>
+      <c r="K6" t="n">
+        <v>2536</v>
+      </c>
+      <c r="L6" t="n">
+        <v>25</v>
+      </c>
+      <c r="M6" t="n">
+        <v>5540</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.95</v>
+      </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>An error occurred. ... KeyError('Date_Uploaded.Data as of')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Tennessee</t>
-        </is>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>44041</v>
-      </c>
-      <c r="C7" t="n">
-        <v>100822</v>
-      </c>
-      <c r="D7" t="n">
-        <v>1020</v>
-      </c>
-      <c r="E7" t="n">
-        <v>19079</v>
-      </c>
-      <c r="F7" t="n">
-        <v>347</v>
-      </c>
-      <c r="G7" t="n">
-        <v>18.92</v>
-      </c>
-      <c r="H7" t="n">
-        <v>34.02</v>
-      </c>
+          <t>NewYork</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr"/>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K7" t="inlineStr"/>
       <c r="L7" t="inlineStr"/>
-      <c r="M7" t="n">
-        <v>1117489</v>
-      </c>
-      <c r="N7" t="n">
-        <v>16.8</v>
-      </c>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
       <c r="O7" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... AssertionError("Key not in dashboard_sections. Valid keys for this data: ['Click Here (Desktop)', 'DASHBOARD 1 DATE (2)', 'Fatalaties by Age Group', 'Fatalaties by County', 'Fatalities by Sex (desktop)', 'PDF Hyperlink (NH)', 'Race', 'Top 10 Comorbid Header', 'Top 10 Comorbidities']")</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Utah</t>
+          <t>New York -- New York</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
@@ -809,43 +741,43 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>39194</t>
+          <t>221220</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>292</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>962</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+          <t>18887</t>
+        </is>
+      </c>
+      <c r="E8" t="n">
+        <v>34191</v>
+      </c>
+      <c r="F8" t="n">
+        <v>5267</v>
       </c>
       <c r="G8" t="n">
-        <v>2.5</v>
+        <v>29.91</v>
       </c>
       <c r="H8" t="n">
-        <v>1.71</v>
+        <v>30.45</v>
       </c>
       <c r="I8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="b">
-        <v>0</v>
-      </c>
-      <c r="K8" t="inlineStr"/>
-      <c r="L8" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K8" t="n">
+        <v>114310</v>
+      </c>
+      <c r="L8" t="n">
+        <v>17298</v>
+      </c>
       <c r="M8" t="n">
-        <v>35862</v>
+        <v>2049418</v>
       </c>
       <c r="N8" t="n">
-        <v>1.18</v>
+        <v>24.27</v>
       </c>
       <c r="O8" t="inlineStr">
         <is>
@@ -856,80 +788,98 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Kentucky</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
-      <c r="E9" t="inlineStr"/>
-      <c r="F9" t="inlineStr"/>
-      <c r="G9" t="inlineStr"/>
-      <c r="H9" t="inlineStr"/>
+          <t>Wisconsin</t>
+        </is>
+      </c>
+      <c r="B9" s="2" t="n">
+        <v>44041</v>
+      </c>
+      <c r="C9" t="n">
+        <v>51049</v>
+      </c>
+      <c r="D9" t="n">
+        <v>911</v>
+      </c>
+      <c r="E9" t="n">
+        <v>7816</v>
+      </c>
+      <c r="F9" t="n">
+        <v>205</v>
+      </c>
+      <c r="G9" t="n">
+        <v>16.95</v>
+      </c>
+      <c r="H9" t="n">
+        <v>22.93</v>
+      </c>
       <c r="I9" t="b">
         <v>0</v>
       </c>
       <c r="J9" t="b">
-        <v>0</v>
-      </c>
-      <c r="K9" t="inlineStr"/>
-      <c r="L9" t="inlineStr"/>
+        <v>1</v>
+      </c>
+      <c r="K9" t="n">
+        <v>46116</v>
+      </c>
+      <c r="L9" t="n">
+        <v>894</v>
+      </c>
       <c r="M9" t="n">
-        <v>354112</v>
+        <v>368744</v>
       </c>
       <c r="N9" t="n">
-        <v>7.98</v>
+        <v>6.38</v>
       </c>
       <c r="O9" t="inlineStr">
         <is>
-          <t>An error occurred. ... AttributeError("'DataFrame' object has no attribute 'str'")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Arkansas</t>
+          <t>Wisconsin -- Milwaukee</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C10" t="n">
-        <v>40968</v>
+        <v>18827</v>
       </c>
       <c r="D10" t="n">
-        <v>434</v>
+        <v>381</v>
       </c>
       <c r="E10" t="n">
-        <v>8673</v>
+        <v>5290</v>
       </c>
       <c r="F10" t="n">
-        <v>113</v>
+        <v>148</v>
       </c>
       <c r="G10" t="n">
-        <v>24.42</v>
+        <v>30.24</v>
       </c>
       <c r="H10" t="n">
-        <v>25.86</v>
+        <v>38.85</v>
       </c>
       <c r="I10" t="b">
         <v>0</v>
       </c>
       <c r="J10" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K10" t="n">
-        <v>35512</v>
+        <v>17494</v>
       </c>
       <c r="L10" t="n">
-        <v>437</v>
+        <v>381</v>
       </c>
       <c r="M10" t="n">
-        <v>460970</v>
+        <v>252321</v>
       </c>
       <c r="N10" t="n">
-        <v>15.41</v>
+        <v>26.44</v>
       </c>
       <c r="O10" t="inlineStr">
         <is>
@@ -940,47 +890,47 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>California - San Diego</t>
+          <t>Oregon</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C11" t="n">
-        <v>28005</v>
+        <v>17721</v>
       </c>
       <c r="D11" t="n">
-        <v>547</v>
+        <v>311</v>
       </c>
       <c r="E11" t="n">
-        <v>1034</v>
+        <v>670</v>
       </c>
       <c r="F11" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="G11" t="n">
-        <v>4.73</v>
+        <v>4.3</v>
       </c>
       <c r="H11" t="n">
-        <v>3.77</v>
+        <v>2.87</v>
       </c>
       <c r="I11" t="b">
         <v>0</v>
       </c>
       <c r="J11" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K11" t="n">
-        <v>21845</v>
+        <v>15595</v>
       </c>
       <c r="L11" t="n">
-        <v>531</v>
+        <v>279</v>
       </c>
       <c r="M11" t="n">
-        <v>166412</v>
+        <v>77789</v>
       </c>
       <c r="N11" t="n">
-        <v>5.04</v>
+        <v>1.91</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -991,43 +941,47 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Virginia</t>
+          <t>Rhode Island</t>
         </is>
       </c>
       <c r="B12" s="2" t="n">
-        <v>44033</v>
+        <v>44015</v>
       </c>
       <c r="C12" t="n">
-        <v>79371</v>
+        <v>16491</v>
       </c>
       <c r="D12" t="n">
-        <v>2048</v>
+        <v>960</v>
       </c>
       <c r="E12" t="n">
-        <v>12922</v>
+        <v>1592</v>
       </c>
       <c r="F12" t="n">
-        <v>483</v>
+        <v>48</v>
       </c>
       <c r="G12" t="n">
-        <v>16.28</v>
+        <v>12.29</v>
       </c>
       <c r="H12" t="n">
-        <v>23.58</v>
+        <v>6.14</v>
       </c>
       <c r="I12" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J12" t="b">
-        <v>1</v>
-      </c>
-      <c r="K12" t="inlineStr"/>
-      <c r="L12" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K12" t="n">
+        <v>12950</v>
+      </c>
+      <c r="L12" t="n">
+        <v>782</v>
+      </c>
       <c r="M12" t="n">
-        <v>1613285</v>
+        <v>69254</v>
       </c>
       <c r="N12" t="n">
-        <v>19.17</v>
+        <v>6.55</v>
       </c>
       <c r="O12" t="inlineStr">
         <is>
@@ -1038,40 +992,44 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>New Mexico</t>
+          <t>SouthCarolina</t>
         </is>
       </c>
       <c r="B13" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C13" t="n">
-        <v>20136</v>
+        <v>84109</v>
       </c>
       <c r="D13" t="n">
-        <v>632</v>
+        <v>1565</v>
       </c>
       <c r="E13" t="n">
-        <v>374</v>
-      </c>
-      <c r="F13" t="inlineStr"/>
+        <v>28332</v>
+      </c>
+      <c r="F13" t="n">
+        <v>642</v>
+      </c>
       <c r="G13" t="n">
-        <v>1.86</v>
-      </c>
-      <c r="H13" t="inlineStr"/>
+        <v>38.21</v>
+      </c>
+      <c r="H13" t="n">
+        <v>43.41</v>
+      </c>
       <c r="I13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
-      </c>
-      <c r="K13" t="inlineStr"/>
-      <c r="L13" t="inlineStr"/>
-      <c r="M13" t="n">
-        <v>43006</v>
-      </c>
-      <c r="N13" t="n">
-        <v>2.06</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K13" t="n">
+        <v>74148</v>
+      </c>
+      <c r="L13" t="n">
+        <v>1479</v>
+      </c>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
       <c r="O13" t="inlineStr">
         <is>
           <t>Success!</t>
@@ -1081,41 +1039,43 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Florida -- Miami-Dade County</t>
+          <t>Tennessee</t>
         </is>
       </c>
       <c r="B14" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C14" t="n">
-        <v>113143</v>
+        <v>100822</v>
       </c>
       <c r="D14" t="n">
-        <v>1455</v>
+        <v>1020</v>
       </c>
       <c r="E14" t="n">
-        <v>10203</v>
-      </c>
-      <c r="F14" t="inlineStr"/>
+        <v>19079</v>
+      </c>
+      <c r="F14" t="n">
+        <v>347</v>
+      </c>
       <c r="G14" t="n">
-        <v>17.58</v>
-      </c>
-      <c r="H14" t="inlineStr"/>
+        <v>18.92</v>
+      </c>
+      <c r="H14" t="n">
+        <v>34.02</v>
+      </c>
       <c r="I14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J14" t="b">
         <v>1</v>
       </c>
-      <c r="K14" t="n">
-        <v>58047</v>
-      </c>
+      <c r="K14" t="inlineStr"/>
       <c r="L14" t="inlineStr"/>
       <c r="M14" t="n">
-        <v>481976</v>
+        <v>1117489</v>
       </c>
       <c r="N14" t="n">
-        <v>17.75</v>
+        <v>16.8</v>
       </c>
       <c r="O14" t="inlineStr">
         <is>
@@ -1126,24 +1086,24 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Florida -- Orange County</t>
+          <t>Maine</t>
         </is>
       </c>
       <c r="B15" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C15" t="n">
-        <v>28191</v>
+        <v>3866</v>
       </c>
       <c r="D15" t="n">
-        <v>203</v>
+        <v>121</v>
       </c>
       <c r="E15" t="n">
-        <v>3659</v>
+        <v>867</v>
       </c>
       <c r="F15" t="inlineStr"/>
       <c r="G15" t="n">
-        <v>25.02</v>
+        <v>24.84</v>
       </c>
       <c r="H15" t="inlineStr"/>
       <c r="I15" t="b">
@@ -1153,14 +1113,14 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
-        <v>14626</v>
+        <v>3490</v>
       </c>
       <c r="L15" t="inlineStr"/>
       <c r="M15" t="n">
-        <v>277193</v>
+        <v>17881</v>
       </c>
       <c r="N15" t="n">
-        <v>20.98</v>
+        <v>1.34</v>
       </c>
       <c r="O15" t="inlineStr">
         <is>
@@ -1171,29 +1131,29 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Alabama</t>
+          <t>Maryland</t>
         </is>
       </c>
       <c r="B16" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C16" t="n">
-        <v>81572</v>
+        <v>86285</v>
       </c>
       <c r="D16" t="n">
-        <v>1489</v>
+        <v>3347</v>
       </c>
       <c r="E16" t="n">
-        <v>23239</v>
+        <v>26189</v>
       </c>
       <c r="F16" t="n">
-        <v>623</v>
+        <v>1365</v>
       </c>
       <c r="G16" t="n">
-        <v>43.04</v>
+        <v>36.45</v>
       </c>
       <c r="H16" t="n">
-        <v>43.41</v>
+        <v>41.1</v>
       </c>
       <c r="I16" t="b">
         <v>0</v>
@@ -1202,16 +1162,16 @@
         <v>0</v>
       </c>
       <c r="K16" t="n">
-        <v>53995</v>
+        <v>71855</v>
       </c>
       <c r="L16" t="n">
-        <v>1435</v>
+        <v>3321</v>
       </c>
       <c r="M16" t="n">
-        <v>1293186</v>
+        <v>1788090</v>
       </c>
       <c r="N16" t="n">
-        <v>26.58</v>
+        <v>29.78</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1222,29 +1182,29 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>California - Los Angeles</t>
+          <t>Alabama</t>
         </is>
       </c>
       <c r="B17" s="2" t="n">
-        <v>44039</v>
+        <v>44041</v>
       </c>
       <c r="C17" t="n">
-        <v>178642</v>
+        <v>81572</v>
       </c>
       <c r="D17" t="n">
-        <v>4426</v>
+        <v>1489</v>
       </c>
       <c r="E17" t="n">
-        <v>4774</v>
+        <v>23239</v>
       </c>
       <c r="F17" t="n">
-        <v>441</v>
+        <v>623</v>
       </c>
       <c r="G17" t="n">
-        <v>4.62</v>
+        <v>43.04</v>
       </c>
       <c r="H17" t="n">
-        <v>10.67</v>
+        <v>43.41</v>
       </c>
       <c r="I17" t="b">
         <v>0</v>
@@ -1253,16 +1213,16 @@
         <v>0</v>
       </c>
       <c r="K17" t="n">
-        <v>103302</v>
+        <v>53995</v>
       </c>
       <c r="L17" t="n">
-        <v>4133</v>
+        <v>1435</v>
       </c>
       <c r="M17" t="n">
-        <v>823987</v>
+        <v>1293186</v>
       </c>
       <c r="N17" t="n">
-        <v>8.16</v>
+        <v>26.58</v>
       </c>
       <c r="O17" t="inlineStr">
         <is>
@@ -1273,47 +1233,47 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Maryland</t>
+          <t>Arkansas</t>
         </is>
       </c>
       <c r="B18" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C18" t="n">
-        <v>86285</v>
+        <v>40968</v>
       </c>
       <c r="D18" t="n">
-        <v>3347</v>
+        <v>434</v>
       </c>
       <c r="E18" t="n">
-        <v>26189</v>
+        <v>8673</v>
       </c>
       <c r="F18" t="n">
-        <v>1365</v>
+        <v>113</v>
       </c>
       <c r="G18" t="n">
-        <v>36.45</v>
+        <v>24.42</v>
       </c>
       <c r="H18" t="n">
-        <v>41.1</v>
+        <v>25.86</v>
       </c>
       <c r="I18" t="b">
         <v>0</v>
       </c>
       <c r="J18" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="n">
-        <v>71855</v>
+        <v>35512</v>
       </c>
       <c r="L18" t="n">
-        <v>3321</v>
+        <v>437</v>
       </c>
       <c r="M18" t="n">
-        <v>1788090</v>
+        <v>460970</v>
       </c>
       <c r="N18" t="n">
-        <v>29.78</v>
+        <v>15.41</v>
       </c>
       <c r="O18" t="inlineStr">
         <is>
@@ -1324,94 +1284,76 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Mississippi</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>44040</v>
-      </c>
-      <c r="C19" t="n">
-        <v>55804</v>
-      </c>
-      <c r="D19" t="n">
-        <v>1563</v>
-      </c>
-      <c r="E19" t="n">
-        <v>24054</v>
-      </c>
-      <c r="F19" t="n">
-        <v>782</v>
-      </c>
-      <c r="G19" t="n">
-        <v>43.1</v>
-      </c>
-      <c r="H19" t="n">
-        <v>50.03</v>
-      </c>
+          <t>Ohio</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+      <c r="E19" t="inlineStr"/>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr"/>
       <c r="I19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="inlineStr"/>
       <c r="L19" t="inlineStr"/>
       <c r="M19" t="n">
-        <v>1125834</v>
+        <v>1438271</v>
       </c>
       <c r="N19" t="n">
-        <v>37.67</v>
+        <v>12.35</v>
       </c>
       <c r="O19" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Arizona</t>
+          <t>Connecticut</t>
         </is>
       </c>
       <c r="B20" s="2" t="n">
-        <v>44041</v>
+        <v>44040</v>
       </c>
       <c r="C20" t="n">
-        <v>168273</v>
+        <v>47581</v>
       </c>
       <c r="D20" t="n">
-        <v>3454</v>
+        <v>3544</v>
       </c>
       <c r="E20" t="n">
-        <v>3822</v>
+        <v>6469</v>
       </c>
       <c r="F20" t="n">
-        <v>104</v>
+        <v>654</v>
       </c>
       <c r="G20" t="n">
-        <v>4.4</v>
+        <v>13.6</v>
       </c>
       <c r="H20" t="n">
-        <v>3.52</v>
+        <v>18.45</v>
       </c>
       <c r="I20" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J20" t="b">
         <v>0</v>
       </c>
-      <c r="K20" t="n">
-        <v>86854</v>
-      </c>
-      <c r="L20" t="n">
-        <v>2951</v>
-      </c>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
       <c r="M20" t="n">
-        <v>305259</v>
+        <v>378262</v>
       </c>
       <c r="N20" t="n">
-        <v>4.39</v>
+        <v>10.56</v>
       </c>
       <c r="O20" t="inlineStr">
         <is>
@@ -1422,47 +1364,43 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Pennsylvania</t>
+          <t>Michigan</t>
         </is>
       </c>
       <c r="B21" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C21" t="n">
-        <v>107138</v>
+        <v>80086</v>
       </c>
       <c r="D21" t="n">
-        <v>7162</v>
+        <v>6094</v>
       </c>
       <c r="E21" t="n">
-        <v>15159</v>
+        <v>22150</v>
       </c>
       <c r="F21" t="n">
-        <v>1484</v>
+        <v>2426</v>
       </c>
       <c r="G21" t="n">
-        <v>29.73</v>
+        <v>27.66</v>
       </c>
       <c r="H21" t="n">
-        <v>21.22</v>
+        <v>39.81</v>
       </c>
       <c r="I21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J21" t="b">
-        <v>1</v>
-      </c>
-      <c r="K21" t="n">
-        <v>50989</v>
-      </c>
-      <c r="L21" t="n">
-        <v>6992</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
       <c r="M21" t="n">
-        <v>1423319</v>
+        <v>1375424</v>
       </c>
       <c r="N21" t="n">
-        <v>11.13</v>
+        <v>13.81</v>
       </c>
       <c r="O21" t="inlineStr">
         <is>
@@ -1473,43 +1411,39 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Florida</t>
+          <t>Montana</t>
         </is>
       </c>
       <c r="B22" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C22" t="n">
-        <v>446251</v>
+        <v>3676</v>
       </c>
       <c r="D22" t="n">
-        <v>6333</v>
+        <v>54</v>
       </c>
       <c r="E22" t="n">
-        <v>53771</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1205</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="n">
-        <v>12.05</v>
-      </c>
-      <c r="H22" t="n">
-        <v>19.03</v>
-      </c>
+        <v>0.57</v>
+      </c>
+      <c r="H22" t="inlineStr"/>
       <c r="I22" t="b">
         <v>1</v>
       </c>
       <c r="J22" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22" t="inlineStr"/>
       <c r="L22" t="inlineStr"/>
       <c r="M22" t="n">
-        <v>3316376</v>
+        <v>4630</v>
       </c>
       <c r="N22" t="n">
-        <v>16.1</v>
+        <v>0.44</v>
       </c>
       <c r="O22" t="inlineStr">
         <is>
@@ -1520,69 +1454,59 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Montana</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>44041</v>
-      </c>
-      <c r="C23" t="n">
-        <v>3676</v>
-      </c>
-      <c r="D23" t="n">
-        <v>54</v>
-      </c>
-      <c r="E23" t="n">
-        <v>21</v>
-      </c>
+          <t>Kansas</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
+      <c r="E23" t="inlineStr"/>
       <c r="F23" t="inlineStr"/>
-      <c r="G23" t="n">
-        <v>0.57</v>
-      </c>
+      <c r="G23" t="inlineStr"/>
       <c r="H23" t="inlineStr"/>
       <c r="I23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J23" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K23" t="inlineStr"/>
       <c r="L23" t="inlineStr"/>
       <c r="M23" t="n">
-        <v>4630</v>
+        <v>169801</v>
       </c>
       <c r="N23" t="n">
-        <v>0.44</v>
+        <v>5.84</v>
       </c>
       <c r="O23" t="inlineStr">
         <is>
-          <t>Success!</t>
+          <t>An error occurred. ... TimeoutException('', None, None)</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Vermont</t>
+          <t>Alaska</t>
         </is>
       </c>
       <c r="B24" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C24" t="n">
-        <v>1406</v>
+        <v>1743</v>
       </c>
       <c r="D24" t="n">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="E24" t="n">
-        <v>160</v>
+        <v>81</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
       </c>
       <c r="G24" t="n">
-        <v>11.71</v>
+        <v>5.06</v>
       </c>
       <c r="H24" t="n">
         <v>0</v>
@@ -1594,16 +1518,16 @@
         <v>1</v>
       </c>
       <c r="K24" t="n">
-        <v>1366</v>
+        <v>1601</v>
       </c>
       <c r="L24" t="n">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="M24" t="n">
-        <v>8058</v>
+        <v>24129</v>
       </c>
       <c r="N24" t="n">
-        <v>1.29</v>
+        <v>3.27</v>
       </c>
       <c r="O24" t="inlineStr">
         <is>
@@ -1614,44 +1538,32 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Connecticut</t>
+          <t>NorthDakota</t>
         </is>
       </c>
       <c r="B25" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C25" t="n">
-        <v>47581</v>
+        <v>6227</v>
       </c>
       <c r="D25" t="n">
-        <v>3544</v>
-      </c>
-      <c r="E25" t="n">
-        <v>6469</v>
-      </c>
-      <c r="F25" t="n">
-        <v>654</v>
-      </c>
-      <c r="G25" t="n">
-        <v>13.6</v>
-      </c>
-      <c r="H25" t="n">
-        <v>18.45</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="E25" t="inlineStr"/>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr"/>
+      <c r="H25" t="inlineStr"/>
       <c r="I25" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25" t="b">
         <v>0</v>
       </c>
       <c r="K25" t="inlineStr"/>
       <c r="L25" t="inlineStr"/>
-      <c r="M25" t="n">
-        <v>378262</v>
-      </c>
-      <c r="N25" t="n">
-        <v>10.56</v>
-      </c>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
       <c r="O25" t="inlineStr">
         <is>
           <t>Success!</t>
@@ -1661,47 +1573,43 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Kansas</t>
+          <t>Massachusetts</t>
         </is>
       </c>
       <c r="B26" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C26" t="n">
-        <v>26870</v>
+        <v>116684</v>
       </c>
       <c r="D26" t="n">
-        <v>349</v>
+        <v>8580</v>
       </c>
       <c r="E26" t="n">
-        <v>2003</v>
+        <v>10934</v>
       </c>
       <c r="F26" t="n">
-        <v>63</v>
+        <v>703</v>
       </c>
       <c r="G26" t="n">
-        <v>9.039999999999999</v>
+        <v>9.369999999999999</v>
       </c>
       <c r="H26" t="n">
-        <v>18.58</v>
+        <v>8.19</v>
       </c>
       <c r="I26" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26" t="b">
-        <v>1</v>
-      </c>
-      <c r="K26" t="n">
-        <v>22161</v>
-      </c>
-      <c r="L26" t="n">
-        <v>339</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
       <c r="M26" t="n">
-        <v>169801</v>
+        <v>510558</v>
       </c>
       <c r="N26" t="n">
-        <v>5.84</v>
+        <v>7.48</v>
       </c>
       <c r="O26" t="inlineStr">
         <is>
@@ -1712,47 +1620,41 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Colorado</t>
+          <t>Florida -- Miami-Dade County</t>
         </is>
       </c>
       <c r="B27" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C27" t="n">
-        <v>45796</v>
+        <v>113143</v>
       </c>
       <c r="D27" t="n">
-        <v>1822</v>
+        <v>1455</v>
       </c>
       <c r="E27" t="n">
-        <v>2130</v>
-      </c>
-      <c r="F27" t="n">
-        <v>121</v>
-      </c>
+        <v>10203</v>
+      </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="n">
-        <v>6.02</v>
-      </c>
-      <c r="H27" t="n">
-        <v>6.87</v>
-      </c>
+        <v>17.58</v>
+      </c>
+      <c r="H27" t="inlineStr"/>
       <c r="I27" t="b">
         <v>0</v>
       </c>
       <c r="J27" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" t="n">
-        <v>35396</v>
-      </c>
-      <c r="L27" t="n">
-        <v>1761</v>
-      </c>
+        <v>58047</v>
+      </c>
+      <c r="L27" t="inlineStr"/>
       <c r="M27" t="n">
-        <v>227938</v>
+        <v>481976</v>
       </c>
       <c r="N27" t="n">
-        <v>4.12</v>
+        <v>17.75</v>
       </c>
       <c r="O27" t="inlineStr">
         <is>
@@ -1763,30 +1665,26 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Nebraska</t>
+          <t>Florida -- Orange County</t>
         </is>
       </c>
       <c r="B28" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C28" t="n">
-        <v>25157</v>
+        <v>28191</v>
       </c>
       <c r="D28" t="n">
-        <v>321</v>
+        <v>203</v>
       </c>
       <c r="E28" t="n">
-        <v>1540</v>
-      </c>
-      <c r="F28" t="n">
-        <v>24</v>
-      </c>
+        <v>3659</v>
+      </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="n">
-        <v>7.85</v>
-      </c>
-      <c r="H28" t="n">
-        <v>7.87</v>
-      </c>
+        <v>25.02</v>
+      </c>
+      <c r="H28" t="inlineStr"/>
       <c r="I28" t="b">
         <v>0</v>
       </c>
@@ -1794,16 +1692,14 @@
         <v>1</v>
       </c>
       <c r="K28" t="n">
-        <v>19625</v>
-      </c>
-      <c r="L28" t="n">
-        <v>305</v>
-      </c>
+        <v>14626</v>
+      </c>
+      <c r="L28" t="inlineStr"/>
       <c r="M28" t="n">
-        <v>90860</v>
+        <v>277193</v>
       </c>
       <c r="N28" t="n">
-        <v>4.77</v>
+        <v>20.98</v>
       </c>
       <c r="O28" t="inlineStr">
         <is>
@@ -1814,43 +1710,43 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Michigan</t>
+          <t>Iowa</t>
         </is>
       </c>
       <c r="B29" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C29" t="n">
-        <v>80086</v>
+        <v>43365</v>
       </c>
       <c r="D29" t="n">
-        <v>6094</v>
+        <v>849</v>
       </c>
       <c r="E29" t="n">
-        <v>22150</v>
+        <v>3419</v>
       </c>
       <c r="F29" t="n">
-        <v>2426</v>
+        <v>38</v>
       </c>
       <c r="G29" t="n">
-        <v>27.66</v>
+        <v>7.88</v>
       </c>
       <c r="H29" t="n">
-        <v>39.81</v>
+        <v>4.48</v>
       </c>
       <c r="I29" t="b">
         <v>1</v>
       </c>
       <c r="J29" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K29" t="inlineStr"/>
       <c r="L29" t="inlineStr"/>
       <c r="M29" t="n">
-        <v>1375424</v>
+        <v>109911</v>
       </c>
       <c r="N29" t="n">
-        <v>13.81</v>
+        <v>3.51</v>
       </c>
       <c r="O29" t="inlineStr">
         <is>
@@ -1861,29 +1757,29 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Louisiana</t>
+          <t>Missouri</t>
         </is>
       </c>
       <c r="B30" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C30" t="n">
-        <v>112773</v>
+        <v>46748</v>
       </c>
       <c r="D30" t="n">
-        <v>3769</v>
+        <v>1220</v>
       </c>
       <c r="E30" t="n">
-        <v>41962</v>
+        <v>9769</v>
       </c>
       <c r="F30" t="n">
-        <v>1884</v>
+        <v>403</v>
       </c>
       <c r="G30" t="n">
-        <v>44.38</v>
+        <v>27.8</v>
       </c>
       <c r="H30" t="n">
-        <v>50.36</v>
+        <v>34.33</v>
       </c>
       <c r="I30" t="b">
         <v>0</v>
@@ -1892,16 +1788,16 @@
         <v>1</v>
       </c>
       <c r="K30" t="n">
-        <v>94556</v>
+        <v>35135</v>
       </c>
       <c r="L30" t="n">
-        <v>3741</v>
+        <v>1174</v>
       </c>
       <c r="M30" t="n">
-        <v>1502916</v>
+        <v>704896</v>
       </c>
       <c r="N30" t="n">
-        <v>32.23</v>
+        <v>11.57</v>
       </c>
       <c r="O30" t="inlineStr">
         <is>
@@ -1912,47 +1808,51 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>California</t>
-        </is>
-      </c>
-      <c r="B31" s="3" t="n">
-        <v>44040</v>
-      </c>
-      <c r="C31" t="n">
-        <v>475305</v>
-      </c>
-      <c r="D31" t="n">
-        <v>8715</v>
-      </c>
-      <c r="E31" t="n">
-        <v>13099</v>
-      </c>
-      <c r="F31" t="n">
-        <v>710</v>
+          <t>Utah</t>
+        </is>
+      </c>
+      <c r="B31" s="2" t="n">
+        <v>44041</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>39194</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>292</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>962</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
       </c>
       <c r="G31" t="n">
-        <v>4.31</v>
+        <v>2.5</v>
       </c>
       <c r="H31" t="n">
-        <v>8.470000000000001</v>
+        <v>1.71</v>
       </c>
       <c r="I31" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31" t="b">
         <v>0</v>
       </c>
-      <c r="K31" t="n">
-        <v>303794</v>
-      </c>
-      <c r="L31" t="n">
-        <v>8379</v>
-      </c>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
       <c r="M31" t="n">
-        <v>2267875</v>
+        <v>35862</v>
       </c>
       <c r="N31" t="n">
-        <v>5.79</v>
+        <v>1.18</v>
       </c>
       <c r="O31" t="inlineStr">
         <is>
@@ -1963,29 +1863,29 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Indiana</t>
+          <t>Mississippi</t>
         </is>
       </c>
       <c r="B32" s="2" t="n">
-        <v>44041</v>
+        <v>44040</v>
       </c>
       <c r="C32" t="n">
-        <v>64299</v>
+        <v>55804</v>
       </c>
       <c r="D32" t="n">
-        <v>2733</v>
+        <v>1563</v>
       </c>
       <c r="E32" t="n">
-        <v>7359</v>
+        <v>24054</v>
       </c>
       <c r="F32" t="n">
-        <v>384</v>
+        <v>782</v>
       </c>
       <c r="G32" t="n">
-        <v>11.44</v>
+        <v>43.1</v>
       </c>
       <c r="H32" t="n">
-        <v>14.05</v>
+        <v>50.03</v>
       </c>
       <c r="I32" t="b">
         <v>1</v>
@@ -1996,10 +1896,10 @@
       <c r="K32" t="inlineStr"/>
       <c r="L32" t="inlineStr"/>
       <c r="M32" t="n">
-        <v>619472</v>
+        <v>1125834</v>
       </c>
       <c r="N32" t="n">
-        <v>9.33</v>
+        <v>37.67</v>
       </c>
       <c r="O32" t="inlineStr">
         <is>
@@ -2010,47 +1910,47 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Alaska</t>
+          <t>Texas -- Bexar County</t>
         </is>
       </c>
       <c r="B33" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C33" t="n">
-        <v>1743</v>
+        <v>38930</v>
       </c>
       <c r="D33" t="n">
-        <v>22</v>
+        <v>342</v>
       </c>
       <c r="E33" t="n">
-        <v>81</v>
+        <v>464</v>
       </c>
       <c r="F33" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="G33" t="n">
-        <v>5.06</v>
+        <v>6.81</v>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>15.32</v>
       </c>
       <c r="I33" t="b">
         <v>0</v>
       </c>
       <c r="J33" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K33" t="n">
-        <v>1601</v>
+        <v>6812</v>
       </c>
       <c r="L33" t="n">
-        <v>22</v>
+        <v>111</v>
       </c>
       <c r="M33" t="n">
-        <v>24129</v>
+        <v>146703</v>
       </c>
       <c r="N33" t="n">
-        <v>3.27</v>
+        <v>7.62</v>
       </c>
       <c r="O33" t="inlineStr">
         <is>
@@ -2061,47 +1961,43 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Wisconsin</t>
+          <t>Minnesota</t>
         </is>
       </c>
       <c r="B34" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C34" t="n">
-        <v>51049</v>
+        <v>52947</v>
       </c>
       <c r="D34" t="n">
-        <v>911</v>
+        <v>1589</v>
       </c>
       <c r="E34" t="n">
-        <v>7816</v>
+        <v>10912</v>
       </c>
       <c r="F34" t="n">
-        <v>205</v>
+        <v>149</v>
       </c>
       <c r="G34" t="n">
-        <v>16.95</v>
+        <v>20.61</v>
       </c>
       <c r="H34" t="n">
-        <v>22.93</v>
+        <v>9.380000000000001</v>
       </c>
       <c r="I34" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" t="b">
         <v>1</v>
       </c>
-      <c r="K34" t="n">
-        <v>46116</v>
-      </c>
-      <c r="L34" t="n">
-        <v>894</v>
-      </c>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
       <c r="M34" t="n">
-        <v>368744</v>
+        <v>342186</v>
       </c>
       <c r="N34" t="n">
-        <v>6.38</v>
+        <v>6.19</v>
       </c>
       <c r="O34" t="inlineStr">
         <is>
@@ -2112,43 +2008,43 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Georgia</t>
+          <t>Texas</t>
         </is>
       </c>
       <c r="B35" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C35" t="n">
-        <v>178323</v>
+        <v>33857</v>
       </c>
       <c r="D35" t="n">
-        <v>3642</v>
+        <v>6190</v>
       </c>
       <c r="E35" t="n">
-        <v>46025</v>
+        <v>4442</v>
       </c>
       <c r="F35" t="n">
-        <v>1645</v>
+        <v>866</v>
       </c>
       <c r="G35" t="n">
-        <v>25.81</v>
+        <v>13.12</v>
       </c>
       <c r="H35" t="n">
-        <v>45.17</v>
+        <v>13.99</v>
       </c>
       <c r="I35" t="b">
         <v>1</v>
       </c>
       <c r="J35" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35" t="inlineStr"/>
       <c r="L35" t="inlineStr"/>
       <c r="M35" t="n">
-        <v>3239300</v>
+        <v>3365783</v>
       </c>
       <c r="N35" t="n">
-        <v>31.46</v>
+        <v>12.07</v>
       </c>
       <c r="O35" t="inlineStr">
         <is>
@@ -2159,29 +2055,29 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Washington</t>
+          <t>Delaware</t>
         </is>
       </c>
       <c r="B36" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C36" t="n">
-        <v>54205</v>
+        <v>14602</v>
       </c>
       <c r="D36" t="n">
-        <v>1548</v>
+        <v>581</v>
       </c>
       <c r="E36" t="n">
-        <v>1984</v>
+        <v>3714</v>
       </c>
       <c r="F36" t="n">
-        <v>49</v>
+        <v>148</v>
       </c>
       <c r="G36" t="n">
-        <v>5.52</v>
+        <v>27.91</v>
       </c>
       <c r="H36" t="n">
-        <v>3.26</v>
+        <v>26.67</v>
       </c>
       <c r="I36" t="b">
         <v>0</v>
@@ -2190,16 +2086,16 @@
         <v>0</v>
       </c>
       <c r="K36" t="n">
-        <v>35958</v>
+        <v>13306</v>
       </c>
       <c r="L36" t="n">
-        <v>1505</v>
+        <v>555</v>
       </c>
       <c r="M36" t="n">
-        <v>269854</v>
+        <v>209892</v>
       </c>
       <c r="N36" t="n">
-        <v>3.7</v>
+        <v>22.11</v>
       </c>
       <c r="O36" t="inlineStr">
         <is>
@@ -2210,47 +2106,47 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>New Hampshire</t>
+          <t>Nebraska</t>
         </is>
       </c>
       <c r="B37" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C37" t="n">
-        <v>6513</v>
+        <v>25422</v>
       </c>
       <c r="D37" t="n">
-        <v>411</v>
+        <v>324</v>
       </c>
       <c r="E37" t="n">
-        <v>338</v>
+        <v>1557</v>
       </c>
       <c r="F37" t="n">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G37" t="n">
-        <v>5.98</v>
+        <v>7.84</v>
       </c>
       <c r="H37" t="n">
-        <v>2.21</v>
+        <v>7.79</v>
       </c>
       <c r="I37" t="b">
         <v>0</v>
       </c>
       <c r="J37" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K37" t="n">
-        <v>5650</v>
+        <v>19862</v>
       </c>
       <c r="L37" t="n">
-        <v>407</v>
+        <v>308</v>
       </c>
       <c r="M37" t="n">
-        <v>20516</v>
+        <v>90860</v>
       </c>
       <c r="N37" t="n">
-        <v>1.53</v>
+        <v>4.77</v>
       </c>
       <c r="O37" t="inlineStr">
         <is>
@@ -2261,43 +2157,47 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Washington, DC</t>
-        </is>
-      </c>
-      <c r="B38" s="2" t="n">
-        <v>44041</v>
+          <t>California</t>
+        </is>
+      </c>
+      <c r="B38" s="3" t="n">
+        <v>44040</v>
       </c>
       <c r="C38" t="n">
-        <v>11999</v>
+        <v>475305</v>
       </c>
       <c r="D38" t="n">
-        <v>584</v>
+        <v>8715</v>
       </c>
       <c r="E38" t="n">
-        <v>5908</v>
+        <v>13099</v>
       </c>
       <c r="F38" t="n">
-        <v>431</v>
+        <v>710</v>
       </c>
       <c r="G38" t="n">
-        <v>49.24</v>
+        <v>4.31</v>
       </c>
       <c r="H38" t="n">
-        <v>73.8</v>
+        <v>8.470000000000001</v>
       </c>
       <c r="I38" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J38" t="b">
-        <v>1</v>
-      </c>
-      <c r="K38" t="inlineStr"/>
-      <c r="L38" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K38" t="n">
+        <v>303794</v>
+      </c>
+      <c r="L38" t="n">
+        <v>8379</v>
+      </c>
       <c r="M38" t="n">
-        <v>321317</v>
+        <v>2267875</v>
       </c>
       <c r="N38" t="n">
-        <v>46.94</v>
+        <v>5.79</v>
       </c>
       <c r="O38" t="inlineStr">
         <is>
@@ -2308,15 +2208,25 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Delaware</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+          <t>SouthDakota</t>
+        </is>
+      </c>
+      <c r="B39" s="2" t="n">
+        <v>44041</v>
+      </c>
+      <c r="C39" t="n">
+        <v>8641</v>
+      </c>
+      <c r="D39" t="n">
+        <v>129</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1016</v>
+      </c>
       <c r="F39" t="inlineStr"/>
-      <c r="G39" t="inlineStr"/>
+      <c r="G39" t="n">
+        <v>11.76</v>
+      </c>
       <c r="H39" t="inlineStr"/>
       <c r="I39" t="b">
         <v>0</v>
@@ -2324,43 +2234,45 @@
       <c r="J39" t="b">
         <v>0</v>
       </c>
-      <c r="K39" t="inlineStr"/>
+      <c r="K39" t="n">
+        <v>8641</v>
+      </c>
       <c r="L39" t="inlineStr"/>
-      <c r="M39" t="n">
-        <v>209892</v>
-      </c>
-      <c r="N39" t="n">
-        <v>22.11</v>
-      </c>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
       <c r="O39" t="inlineStr">
         <is>
-          <t>An error occurred. ... WebDriverException('unknown error: session deleted because of page crash\nfrom unknown error: cannot determine loading status\nfrom tab crashed\n  (Session info: headless chrome=83.0.4103.116)', None, None)</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Maine</t>
+          <t>Vermont</t>
         </is>
       </c>
       <c r="B40" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C40" t="n">
-        <v>3866</v>
+        <v>1406</v>
       </c>
       <c r="D40" t="n">
-        <v>121</v>
+        <v>56</v>
       </c>
       <c r="E40" t="n">
-        <v>867</v>
-      </c>
-      <c r="F40" t="inlineStr"/>
+        <v>160</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
       <c r="G40" t="n">
-        <v>24.84</v>
-      </c>
-      <c r="H40" t="inlineStr"/>
+        <v>11.71</v>
+      </c>
+      <c r="H40" t="n">
+        <v>0</v>
+      </c>
       <c r="I40" t="b">
         <v>0</v>
       </c>
@@ -2368,14 +2280,16 @@
         <v>1</v>
       </c>
       <c r="K40" t="n">
-        <v>3490</v>
-      </c>
-      <c r="L40" t="inlineStr"/>
+        <v>1366</v>
+      </c>
+      <c r="L40" t="n">
+        <v>56</v>
+      </c>
       <c r="M40" t="n">
-        <v>17881</v>
+        <v>8058</v>
       </c>
       <c r="N40" t="n">
-        <v>1.34</v>
+        <v>1.29</v>
       </c>
       <c r="O40" t="inlineStr">
         <is>
@@ -2386,43 +2300,39 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Iowa</t>
+          <t>New Mexico</t>
         </is>
       </c>
       <c r="B41" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C41" t="n">
-        <v>43283</v>
+        <v>20136</v>
       </c>
       <c r="D41" t="n">
-        <v>846</v>
+        <v>632</v>
       </c>
       <c r="E41" t="n">
-        <v>3415</v>
-      </c>
-      <c r="F41" t="n">
-        <v>38</v>
-      </c>
+        <v>374</v>
+      </c>
+      <c r="F41" t="inlineStr"/>
       <c r="G41" t="n">
-        <v>7.89</v>
-      </c>
-      <c r="H41" t="n">
-        <v>4.49</v>
-      </c>
+        <v>1.86</v>
+      </c>
+      <c r="H41" t="inlineStr"/>
       <c r="I41" t="b">
         <v>1</v>
       </c>
       <c r="J41" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K41" t="inlineStr"/>
       <c r="L41" t="inlineStr"/>
       <c r="M41" t="n">
-        <v>109911</v>
+        <v>43006</v>
       </c>
       <c r="N41" t="n">
-        <v>3.51</v>
+        <v>2.06</v>
       </c>
       <c r="O41" t="inlineStr">
         <is>
@@ -2433,47 +2343,43 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>North Carolina</t>
+          <t>Florida</t>
         </is>
       </c>
       <c r="B42" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C42" t="n">
-        <v>117850</v>
+        <v>446251</v>
       </c>
       <c r="D42" t="n">
-        <v>1865</v>
+        <v>6333</v>
       </c>
       <c r="E42" t="n">
-        <v>20252</v>
+        <v>53771</v>
       </c>
       <c r="F42" t="n">
-        <v>576</v>
+        <v>1205</v>
       </c>
       <c r="G42" t="n">
-        <v>24.04</v>
+        <v>12.05</v>
       </c>
       <c r="H42" t="n">
-        <v>31.96</v>
+        <v>19.03</v>
       </c>
       <c r="I42" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42" t="b">
-        <v>1</v>
-      </c>
-      <c r="K42" t="n">
-        <v>84258</v>
-      </c>
-      <c r="L42" t="n">
-        <v>1802</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
       <c r="M42" t="n">
-        <v>2179622</v>
+        <v>3316376</v>
       </c>
       <c r="N42" t="n">
-        <v>21.46</v>
+        <v>16.1</v>
       </c>
       <c r="O42" t="inlineStr">
         <is>
@@ -2484,43 +2390,43 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Illinois</t>
+          <t>Washington, DC</t>
         </is>
       </c>
       <c r="B43" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C43" t="n">
-        <v>175124</v>
+        <v>11999</v>
       </c>
       <c r="D43" t="n">
-        <v>7462</v>
+        <v>584</v>
       </c>
       <c r="E43" t="n">
-        <v>29105</v>
+        <v>5908</v>
       </c>
       <c r="F43" t="n">
-        <v>2045</v>
+        <v>431</v>
       </c>
       <c r="G43" t="n">
-        <v>16.62</v>
+        <v>49.24</v>
       </c>
       <c r="H43" t="n">
-        <v>27.41</v>
+        <v>73.8</v>
       </c>
       <c r="I43" t="b">
         <v>1</v>
       </c>
       <c r="J43" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K43" t="inlineStr"/>
       <c r="L43" t="inlineStr"/>
       <c r="M43" t="n">
-        <v>1824125</v>
+        <v>321317</v>
       </c>
       <c r="N43" t="n">
-        <v>14.23</v>
+        <v>46.94</v>
       </c>
       <c r="O43" t="inlineStr">
         <is>
@@ -2531,44 +2437,44 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Idaho</t>
+          <t>California - San Francisco</t>
         </is>
       </c>
       <c r="B44" s="2" t="n">
-        <v>44040</v>
+        <v>44038</v>
       </c>
       <c r="C44" t="n">
-        <v>19222</v>
+        <v>6197</v>
       </c>
       <c r="D44" t="n">
-        <v>158</v>
+        <v>57</v>
       </c>
       <c r="E44" t="n">
-        <v>228</v>
+        <v>357</v>
       </c>
       <c r="F44" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G44" t="n">
-        <v>1.19</v>
+        <v>6.74</v>
       </c>
       <c r="H44" t="n">
-        <v>1.9</v>
+        <v>10.71</v>
       </c>
       <c r="I44" t="b">
         <v>0</v>
       </c>
       <c r="J44" t="b">
-        <v>1</v>
-      </c>
-      <c r="K44" t="inlineStr"/>
-      <c r="L44" t="inlineStr"/>
-      <c r="M44" t="n">
-        <v>11536</v>
-      </c>
-      <c r="N44" t="n">
-        <v>0.68</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="K44" t="n">
+        <v>5293</v>
+      </c>
+      <c r="L44" t="n">
+        <v>56</v>
+      </c>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
       <c r="O44" t="inlineStr">
         <is>
           <t>Success!</t>
@@ -2578,76 +2484,98 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Ohio</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr"/>
-      <c r="C45" t="inlineStr"/>
-      <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
-      <c r="F45" t="inlineStr"/>
-      <c r="G45" t="inlineStr"/>
-      <c r="H45" t="inlineStr"/>
+          <t>Colorado</t>
+        </is>
+      </c>
+      <c r="B45" s="2" t="n">
+        <v>44041</v>
+      </c>
+      <c r="C45" t="n">
+        <v>45796</v>
+      </c>
+      <c r="D45" t="n">
+        <v>1822</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2130</v>
+      </c>
+      <c r="F45" t="n">
+        <v>121</v>
+      </c>
+      <c r="G45" t="n">
+        <v>6.02</v>
+      </c>
+      <c r="H45" t="n">
+        <v>6.87</v>
+      </c>
       <c r="I45" t="b">
         <v>0</v>
       </c>
       <c r="J45" t="b">
         <v>0</v>
       </c>
-      <c r="K45" t="inlineStr"/>
-      <c r="L45" t="inlineStr"/>
+      <c r="K45" t="n">
+        <v>35396</v>
+      </c>
+      <c r="L45" t="n">
+        <v>1761</v>
+      </c>
       <c r="M45" t="n">
-        <v>1438271</v>
+        <v>227938</v>
       </c>
       <c r="N45" t="n">
-        <v>12.35</v>
+        <v>4.12</v>
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Minnesota</t>
+          <t>California - San Diego</t>
         </is>
       </c>
       <c r="B46" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C46" t="n">
-        <v>52947</v>
+        <v>28287</v>
       </c>
       <c r="D46" t="n">
-        <v>1589</v>
+        <v>552</v>
       </c>
       <c r="E46" t="n">
-        <v>10912</v>
+        <v>1055</v>
       </c>
       <c r="F46" t="n">
-        <v>149</v>
+        <v>21</v>
       </c>
       <c r="G46" t="n">
-        <v>20.61</v>
+        <v>4.73</v>
       </c>
       <c r="H46" t="n">
-        <v>9.380000000000001</v>
+        <v>3.92</v>
       </c>
       <c r="I46" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J46" t="b">
-        <v>1</v>
-      </c>
-      <c r="K46" t="inlineStr"/>
-      <c r="L46" t="inlineStr"/>
+        <v>0</v>
+      </c>
+      <c r="K46" t="n">
+        <v>22283</v>
+      </c>
+      <c r="L46" t="n">
+        <v>536</v>
+      </c>
       <c r="M46" t="n">
-        <v>342186</v>
+        <v>166412</v>
       </c>
       <c r="N46" t="n">
-        <v>6.19</v>
+        <v>5.04</v>
       </c>
       <c r="O46" t="inlineStr">
         <is>
@@ -2658,43 +2586,43 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Massachusetts</t>
+          <t>Idaho</t>
         </is>
       </c>
       <c r="B47" s="2" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="C47" t="n">
-        <v>116182</v>
+        <v>19679</v>
       </c>
       <c r="D47" t="n">
-        <v>8551</v>
+        <v>170</v>
       </c>
       <c r="E47" t="n">
-        <v>10870</v>
+        <v>236</v>
       </c>
       <c r="F47" t="n">
-        <v>700</v>
+        <v>3</v>
       </c>
       <c r="G47" t="n">
-        <v>9.359999999999999</v>
+        <v>1.2</v>
       </c>
       <c r="H47" t="n">
-        <v>8.19</v>
+        <v>1.76</v>
       </c>
       <c r="I47" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J47" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K47" t="inlineStr"/>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="n">
-        <v>510558</v>
+        <v>11536</v>
       </c>
       <c r="N47" t="n">
-        <v>7.48</v>
+        <v>0.68</v>
       </c>
       <c r="O47" t="inlineStr">
         <is>
@@ -2705,47 +2633,47 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Wisconsin -- Milwaukee</t>
+          <t>Pennsylvania</t>
         </is>
       </c>
       <c r="B48" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C48" t="n">
-        <v>18827</v>
+        <v>107138</v>
       </c>
       <c r="D48" t="n">
-        <v>381</v>
+        <v>7162</v>
       </c>
       <c r="E48" t="n">
-        <v>5290</v>
+        <v>15159</v>
       </c>
       <c r="F48" t="n">
-        <v>148</v>
+        <v>1484</v>
       </c>
       <c r="G48" t="n">
-        <v>30.24</v>
+        <v>29.73</v>
       </c>
       <c r="H48" t="n">
-        <v>38.85</v>
+        <v>21.22</v>
       </c>
       <c r="I48" t="b">
         <v>0</v>
       </c>
       <c r="J48" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48" t="n">
-        <v>17494</v>
+        <v>50989</v>
       </c>
       <c r="L48" t="n">
-        <v>381</v>
+        <v>6992</v>
       </c>
       <c r="M48" t="n">
-        <v>252321</v>
+        <v>1423319</v>
       </c>
       <c r="N48" t="n">
-        <v>26.44</v>
+        <v>11.13</v>
       </c>
       <c r="O48" t="inlineStr">
         <is>
@@ -2756,47 +2684,47 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Missouri</t>
+          <t>Arizona</t>
         </is>
       </c>
       <c r="B49" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C49" t="n">
-        <v>46748</v>
+        <v>168273</v>
       </c>
       <c r="D49" t="n">
-        <v>1220</v>
+        <v>3454</v>
       </c>
       <c r="E49" t="n">
-        <v>9769</v>
+        <v>3822</v>
       </c>
       <c r="F49" t="n">
-        <v>403</v>
+        <v>104</v>
       </c>
       <c r="G49" t="n">
-        <v>27.8</v>
+        <v>4.4</v>
       </c>
       <c r="H49" t="n">
-        <v>34.33</v>
+        <v>3.52</v>
       </c>
       <c r="I49" t="b">
         <v>0</v>
       </c>
       <c r="J49" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K49" t="n">
-        <v>35135</v>
+        <v>86854</v>
       </c>
       <c r="L49" t="n">
-        <v>1174</v>
+        <v>2951</v>
       </c>
       <c r="M49" t="n">
-        <v>704896</v>
+        <v>305259</v>
       </c>
       <c r="N49" t="n">
-        <v>11.57</v>
+        <v>4.39</v>
       </c>
       <c r="O49" t="inlineStr">
         <is>
@@ -2807,100 +2735,138 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>NewYork</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr"/>
-      <c r="C50" t="inlineStr"/>
-      <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
-      <c r="F50" t="inlineStr"/>
-      <c r="G50" t="inlineStr"/>
-      <c r="H50" t="inlineStr"/>
+          <t>Georgia</t>
+        </is>
+      </c>
+      <c r="B50" s="2" t="n">
+        <v>44041</v>
+      </c>
+      <c r="C50" t="n">
+        <v>178323</v>
+      </c>
+      <c r="D50" t="n">
+        <v>3642</v>
+      </c>
+      <c r="E50" t="n">
+        <v>46025</v>
+      </c>
+      <c r="F50" t="n">
+        <v>1645</v>
+      </c>
+      <c r="G50" t="n">
+        <v>25.81</v>
+      </c>
+      <c r="H50" t="n">
+        <v>45.17</v>
+      </c>
       <c r="I50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J50" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K50" t="inlineStr"/>
       <c r="L50" t="inlineStr"/>
-      <c r="M50" t="inlineStr"/>
-      <c r="N50" t="inlineStr"/>
+      <c r="M50" t="n">
+        <v>3239300</v>
+      </c>
+      <c r="N50" t="n">
+        <v>31.46</v>
+      </c>
       <c r="O50" t="inlineStr">
         <is>
-          <t>An error occurred. ... AssertionError("Key not in dashboard_sections. Valid keys for this data: ['Click Here (Desktop)', 'DASHBOARD 1 DATE (2)', 'Fatalaties by Age Group', 'Fatalaties by County', 'Fatalities by Sex (desktop)', 'PDF Hyperlink (NH)', 'Race', 'Top 10 Comorbid Header', 'Top 10 Comorbidities']")</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Wyoming</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr"/>
-      <c r="C51" t="inlineStr"/>
-      <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
-      <c r="F51" t="inlineStr"/>
-      <c r="G51" t="inlineStr"/>
-      <c r="H51" t="inlineStr"/>
+          <t>Virginia</t>
+        </is>
+      </c>
+      <c r="B51" s="2" t="n">
+        <v>44033</v>
+      </c>
+      <c r="C51" t="n">
+        <v>79371</v>
+      </c>
+      <c r="D51" t="n">
+        <v>2048</v>
+      </c>
+      <c r="E51" t="n">
+        <v>12922</v>
+      </c>
+      <c r="F51" t="n">
+        <v>483</v>
+      </c>
+      <c r="G51" t="n">
+        <v>16.28</v>
+      </c>
+      <c r="H51" t="n">
+        <v>23.58</v>
+      </c>
       <c r="I51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J51" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K51" t="inlineStr"/>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="n">
-        <v>5540</v>
+        <v>1613285</v>
       </c>
       <c r="N51" t="n">
-        <v>0.95</v>
+        <v>19.17</v>
       </c>
       <c r="O51" t="inlineStr">
         <is>
-          <t>An error occurred. ... JSONDecodeError('Expecting value: line 1 column 1 (char 0)')</t>
+          <t>Success!</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>SouthDakota</t>
+          <t>Indiana</t>
         </is>
       </c>
       <c r="B52" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C52" t="n">
-        <v>8641</v>
+        <v>64299</v>
       </c>
       <c r="D52" t="n">
-        <v>129</v>
+        <v>2733</v>
       </c>
       <c r="E52" t="n">
-        <v>1016</v>
-      </c>
-      <c r="F52" t="inlineStr"/>
+        <v>7359</v>
+      </c>
+      <c r="F52" t="n">
+        <v>384</v>
+      </c>
       <c r="G52" t="n">
-        <v>11.76</v>
-      </c>
-      <c r="H52" t="inlineStr"/>
+        <v>11.44</v>
+      </c>
+      <c r="H52" t="n">
+        <v>14.05</v>
+      </c>
       <c r="I52" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J52" t="b">
-        <v>0</v>
-      </c>
-      <c r="K52" t="n">
-        <v>8641</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="K52" t="inlineStr"/>
       <c r="L52" t="inlineStr"/>
-      <c r="M52" t="inlineStr"/>
-      <c r="N52" t="inlineStr"/>
+      <c r="M52" t="n">
+        <v>619472</v>
+      </c>
+      <c r="N52" t="n">
+        <v>9.33</v>
+      </c>
       <c r="O52" t="inlineStr">
         <is>
           <t>Success!</t>
@@ -2910,45 +2876,133 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>SouthCarolina</t>
+          <t>New Hampshire</t>
         </is>
       </c>
       <c r="B53" s="2" t="n">
         <v>44041</v>
       </c>
       <c r="C53" t="n">
-        <v>84109</v>
+        <v>6513</v>
       </c>
       <c r="D53" t="n">
-        <v>1565</v>
+        <v>411</v>
       </c>
       <c r="E53" t="n">
-        <v>28332</v>
+        <v>338</v>
       </c>
       <c r="F53" t="n">
-        <v>642</v>
+        <v>9</v>
       </c>
       <c r="G53" t="n">
-        <v>38.21</v>
+        <v>5.98</v>
       </c>
       <c r="H53" t="n">
-        <v>43.41</v>
+        <v>2.21</v>
       </c>
       <c r="I53" t="b">
         <v>0</v>
       </c>
       <c r="J53" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K53" t="n">
-        <v>74148</v>
+        <v>5650</v>
       </c>
       <c r="L53" t="n">
-        <v>1479</v>
-      </c>
-      <c r="M53" t="inlineStr"/>
-      <c r="N53" t="inlineStr"/>
+        <v>407</v>
+      </c>
+      <c r="M53" t="n">
+        <v>20516</v>
+      </c>
+      <c r="N53" t="n">
+        <v>1.53</v>
+      </c>
       <c r="O53" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Kentucky</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr"/>
+      <c r="C54" t="inlineStr"/>
+      <c r="D54" t="inlineStr"/>
+      <c r="E54" t="inlineStr"/>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="b">
+        <v>0</v>
+      </c>
+      <c r="J54" t="b">
+        <v>0</v>
+      </c>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="n">
+        <v>354112</v>
+      </c>
+      <c r="N54" t="n">
+        <v>7.98</v>
+      </c>
+      <c r="O54" t="inlineStr">
+        <is>
+          <t>An error occurred. ... AttributeError("'DataFrame' object has no attribute 'str'")</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>California - Los Angeles</t>
+        </is>
+      </c>
+      <c r="B55" s="2" t="n">
+        <v>44040</v>
+      </c>
+      <c r="C55" t="n">
+        <v>183383</v>
+      </c>
+      <c r="D55" t="n">
+        <v>4516</v>
+      </c>
+      <c r="E55" t="n">
+        <v>4907</v>
+      </c>
+      <c r="F55" t="n">
+        <v>449</v>
+      </c>
+      <c r="G55" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="H55" t="n">
+        <v>10.63</v>
+      </c>
+      <c r="I55" t="b">
+        <v>0</v>
+      </c>
+      <c r="J55" t="b">
+        <v>0</v>
+      </c>
+      <c r="K55" t="n">
+        <v>106755</v>
+      </c>
+      <c r="L55" t="n">
+        <v>4223</v>
+      </c>
+      <c r="M55" t="n">
+        <v>823987</v>
+      </c>
+      <c r="N55" t="n">
+        <v>8.16</v>
+      </c>
+      <c r="O55" t="inlineStr">
         <is>
           <t>Success!</t>
         </is>

</xml_diff>